<commit_message>
Correct NGSI-LD attribute names
</commit_message>
<xml_diff>
--- a/ressources/1/export_groups_and_meaning.xlsx
+++ b/ressources/1/export_groups_and_meaning.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,10 +501,15 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>Cleaned_KKS_name</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>OpenAPI_3.0_Type</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>X-NGSI-LD</t>
         </is>
@@ -574,10 +579,15 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0GCN10AP010:WAB_DosPu_NH4OH:SPOP_HL</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -647,10 +657,15 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0GCN10AP010:WAB_DosPu_NH4OH:FB_SPEED</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -720,10 +735,15 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0GCN10AP010:WAB_DosPu_NH4OH:SP_AUT</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -793,10 +813,15 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0GCN10AP010:WAB_DosPu_NH4OH:SP_GRAD</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -866,10 +891,15 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0GCN10AP010:WAB_DosPu_NH4OH:SP_OP</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -939,10 +969,15 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
+          <t>0GCN10AP010:WAB_DosPu_NH4OH:SP_RAMP</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
           <t>boolean</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>https://schema.org/Boolean</t>
         </is>
@@ -1012,10 +1047,15 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0GCN10AP010:WAB_DosPu_NH4OH:SPOP_LL</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -1085,10 +1125,15 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0GHC20AA001:NivRV_SpWB:FB_MV</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -1158,10 +1203,15 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0HLA11DT021:T_RegAustrAbs_MW:IN13</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -1231,10 +1281,15 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0HLA11DT021:T_RegAustrAbs_MW:IN12</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -1304,10 +1359,15 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0HLA11DT021:T_RegAustrAbs_MW:IN16</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -1377,10 +1437,15 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0HLA11DT021:T_RegAustrAbs_MW:IN15</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -1450,10 +1515,15 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0HLA11DT021:T_RegAustrAbs_MW:IN14</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -1523,10 +1593,15 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX99CT910:MWtTempObFlaRec:U_WL</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -1600,10 +1675,15 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX99CT910A:MAXWtTempRec:U</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -1673,10 +1753,15 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX99CT910:MWtTempObFlaRec:U_WH</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -1746,10 +1831,15 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX99CT910:MWtTempObFlaRec:U_AL</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -1819,10 +1909,15 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX99CT910:MWtTempObFlaRec:U_AH</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -1896,10 +1991,15 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX50CT001B:TempHoriTrennRec:U</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -1973,10 +2073,15 @@
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX99CT910A:SP_T_Rec_Grad_D1:U</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -2046,10 +2151,15 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX99CT910:MWtTempObFlaRec:U</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -2123,10 +2233,15 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX99CT910A:SP_T_Rec_Grad_D2:U</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -2200,10 +2315,15 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX99CT910A:SP_T_Rec_Grad_WH:U</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -2277,10 +2397,15 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX99CT940B:MAXTDiff_TrgRah:U</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -2354,10 +2479,15 @@
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX99CT940C:MAXTDiff_KuLuAus:U</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -2431,10 +2561,15 @@
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX99CT910A:MWtTempRec:U</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -2504,10 +2639,15 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX99CT910:MAXWtTempObFlaRe:U_WL</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -2581,10 +2721,15 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX99CT950C:MAXTDiff_KuLu_WL:U</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -2654,10 +2799,15 @@
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX99CT910:MAXWtTempObFlaRe:U_AL</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -2727,10 +2877,15 @@
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX99CT910:MAXWtTempObFlaRe:U_AH</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -2800,10 +2955,15 @@
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX99CT910:MAXWtTempObFlaRe:U</t>
         </is>
       </c>
       <c r="O32" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -2877,10 +3037,15 @@
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX50CT901B:MAXTempTrennRec:U</t>
         </is>
       </c>
       <c r="O33" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -2954,10 +3119,15 @@
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX50CT002B:TempVertTrennRec:U</t>
         </is>
       </c>
       <c r="O34" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -3031,10 +3201,15 @@
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX99CT950B:MAXTDiff_Rah_Mem:U</t>
         </is>
       </c>
       <c r="O35" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P35" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -3108,10 +3283,15 @@
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX30CT901C:MAXT_KuKanSeWdLu:U</t>
         </is>
       </c>
       <c r="O36" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -3181,10 +3361,15 @@
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0WTX99CT910:MAXWtTempObFlaRe:U_WH</t>
         </is>
       </c>
       <c r="O37" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -3254,10 +3439,15 @@
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>number</t>
+          <t xml:space="preserve">0BLE10CS002:Drehzahl_DT:U_WL </t>
         </is>
       </c>
       <c r="O38" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -3327,10 +3517,15 @@
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>number</t>
+          <t xml:space="preserve">0BLE10CS002:Drehzahl_DT:U_WH </t>
         </is>
       </c>
       <c r="O39" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -3400,10 +3595,15 @@
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>number</t>
+          <t xml:space="preserve">0BLE10CS002:Drehzahl_DT:U_AH </t>
         </is>
       </c>
       <c r="O40" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -3473,10 +3673,15 @@
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0BLE10CS002:Drehzahl_DT:U</t>
         </is>
       </c>
       <c r="O41" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P41" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -3546,10 +3751,15 @@
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0HAH20CT002:T_DamAusUebHitz2:PV_IN</t>
         </is>
       </c>
       <c r="O42" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -3619,10 +3829,15 @@
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0HAH20CT002:T_DamAusUebHitz2:LMN</t>
         </is>
       </c>
       <c r="O43" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P43" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>
@@ -3692,10 +3907,15 @@
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>0GKA10CF501:DurFl_RoWa_:ZAEHLWERT</t>
         </is>
       </c>
       <c r="O44" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr">
         <is>
           <t>https://schema.org/Number</t>
         </is>

</xml_diff>